<commit_message>
TP3 Modelos y simulaciones
</commit_message>
<xml_diff>
--- a/5° Año/1° Semestre/Modelos y simulacion/Mario Molina Estocastica/Pyhton/Soria - football - TP2.xlsx
+++ b/5° Año/1° Semestre/Modelos y simulacion/Mario Molina Estocastica/Pyhton/Soria - football - TP2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,13 +471,13 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>1.767766952966369</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.4877258050403206</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1.669766952966369</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -485,128 +485,534 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.419417382415922</v>
+        <v>3.535533905932737</v>
       </c>
       <c r="B4" t="n">
-        <v>1.219314512600802</v>
+        <v>0.9754516100806413</v>
       </c>
       <c r="C4" t="n">
-        <v>4.113167382415921</v>
+        <v>3.241533905932738</v>
       </c>
       <c r="D4" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8.838834764831844</v>
+        <v>5.303300858899106</v>
       </c>
       <c r="B5" t="n">
-        <v>2.438629025201603</v>
+        <v>1.463177415120962</v>
       </c>
       <c r="C5" t="n">
-        <v>7.613834764831843</v>
+        <v>4.715300858899107</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>13.25825214724777</v>
+        <v>7.071067811865475</v>
       </c>
       <c r="B6" t="n">
-        <v>3.657943537802405</v>
+        <v>1.950903220161283</v>
       </c>
       <c r="C6" t="n">
-        <v>10.50200214724776</v>
+        <v>6.091067811865476</v>
       </c>
       <c r="D6" t="n">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>17.67766952966369</v>
+        <v>8.838834764831843</v>
       </c>
       <c r="B7" t="n">
-        <v>4.877258050403206</v>
+        <v>2.438629025201603</v>
       </c>
       <c r="C7" t="n">
-        <v>12.77766952966368</v>
+        <v>7.368834764831845</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>22.09708691207961</v>
+        <v>10.60660171779821</v>
       </c>
       <c r="B8" t="n">
-        <v>6.096572563004008</v>
+        <v>2.926354830241924</v>
       </c>
       <c r="C8" t="n">
-        <v>14.44083691207961</v>
+        <v>8.548601717798213</v>
       </c>
       <c r="D8" t="n">
-        <v>1.25</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>26.51650429449553</v>
+        <v>12.37436867076458</v>
       </c>
       <c r="B9" t="n">
-        <v>7.31588707560481</v>
+        <v>3.414080635282245</v>
       </c>
       <c r="C9" t="n">
-        <v>15.49150429449553</v>
+        <v>9.630368670764582</v>
       </c>
       <c r="D9" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>30.93592167691146</v>
+        <v>14.14213562373095</v>
       </c>
       <c r="B10" t="n">
-        <v>8.535201588205611</v>
+        <v>3.901806440322566</v>
       </c>
       <c r="C10" t="n">
-        <v>15.92967167691145</v>
+        <v>10.61413562373095</v>
       </c>
       <c r="D10" t="n">
-        <v>1.75</v>
+        <v>0.6000000000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>35.35533905932738</v>
+        <v>15.04488810900642</v>
       </c>
       <c r="B11" t="n">
-        <v>9.754516100806413</v>
+        <v>3.948785359893499</v>
       </c>
       <c r="C11" t="n">
-        <v>15.75533905932737</v>
+        <v>11.49990257669732</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>0.7000000000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>39.7747564417433</v>
+        <v>15.082626126591</v>
       </c>
       <c r="B12" t="n">
-        <v>10.97383061340721</v>
+        <v>3.555017393995045</v>
       </c>
       <c r="C12" t="n">
-        <v>14.96850644174329</v>
+        <v>12.28766952966369</v>
       </c>
       <c r="D12" t="n">
-        <v>2.25</v>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>14.25534967648468</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.720502542627205</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12.97743648263006</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.42807322637836</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.885987691259364</v>
+      </c>
+      <c r="C14" t="n">
+        <v>13.56920343559642</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>12.60079677627204</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1.051472839891523</v>
+      </c>
+      <c r="C15" t="n">
+        <v>14.06297038856279</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>11.77352032616572</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.2169579885236828</v>
+      </c>
+      <c r="C16" t="n">
+        <v>14.45873734152916</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>10.9462438760594</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-0.6175568628441579</v>
+      </c>
+      <c r="C17" t="n">
+        <v>14.75650429449553</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>10.11896742595308</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-1.452071714211999</v>
+      </c>
+      <c r="C18" t="n">
+        <v>14.9562712474619</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>9.291690975846761</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-2.286586565579839</v>
+      </c>
+      <c r="C19" t="n">
+        <v>15.05803820042827</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>8.464414525740441</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-3.12110141694768</v>
+      </c>
+      <c r="C20" t="n">
+        <v>15.06180515339463</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>7.637138075634122</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-3.95561626831552</v>
+      </c>
+      <c r="C21" t="n">
+        <v>14.967572106361</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>6.809861625527803</v>
+      </c>
+      <c r="B22" t="n">
+        <v>-4.790131119683361</v>
+      </c>
+      <c r="C22" t="n">
+        <v>14.77533905932737</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>5.982585175421485</v>
+      </c>
+      <c r="B23" t="n">
+        <v>-5.624645971051201</v>
+      </c>
+      <c r="C23" t="n">
+        <v>14.48510601229374</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>5.155308725315166</v>
+      </c>
+      <c r="B24" t="n">
+        <v>-6.459160822419042</v>
+      </c>
+      <c r="C24" t="n">
+        <v>14.09687296526011</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>4.328032275208847</v>
+      </c>
+      <c r="B25" t="n">
+        <v>-7.293675673786883</v>
+      </c>
+      <c r="C25" t="n">
+        <v>13.61063991822647</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3.500755825102528</v>
+      </c>
+      <c r="B26" t="n">
+        <v>-8.128190525154723</v>
+      </c>
+      <c r="C26" t="n">
+        <v>13.02640687119284</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.67347937499621</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-8.962705376522564</v>
+      </c>
+      <c r="C27" t="n">
+        <v>12.34417382415921</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1.846202924889891</v>
+      </c>
+      <c r="B28" t="n">
+        <v>-9.797220227890405</v>
+      </c>
+      <c r="C28" t="n">
+        <v>11.56394077712558</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1.018926474783572</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-10.63173507925825</v>
+      </c>
+      <c r="C29" t="n">
+        <v>10.68570773009194</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.1916500246772526</v>
+      </c>
+      <c r="B30" t="n">
+        <v>-11.46624993062609</v>
+      </c>
+      <c r="C30" t="n">
+        <v>9.709474683058312</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>-0.6356264254290664</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-12.30076478199393</v>
+      </c>
+      <c r="C31" t="n">
+        <v>8.635241636024681</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>-1.462902875535385</v>
+      </c>
+      <c r="B32" t="n">
+        <v>-13.13527963336177</v>
+      </c>
+      <c r="C32" t="n">
+        <v>7.463008588991048</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>-2.290179325641704</v>
+      </c>
+      <c r="B33" t="n">
+        <v>-13.96979448472961</v>
+      </c>
+      <c r="C33" t="n">
+        <v>6.192775541957416</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>-3.117455775748024</v>
+      </c>
+      <c r="B34" t="n">
+        <v>-14.80430933609745</v>
+      </c>
+      <c r="C34" t="n">
+        <v>4.824542494923783</v>
+      </c>
+      <c r="D34" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>-3.944732225854342</v>
+      </c>
+      <c r="B35" t="n">
+        <v>-15.63882418746529</v>
+      </c>
+      <c r="C35" t="n">
+        <v>3.35830944789015</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>-4.772008675960661</v>
+      </c>
+      <c r="B36" t="n">
+        <v>-16.47333903883313</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1.794076400856517</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>-5.59928512606698</v>
+      </c>
+      <c r="B37" t="n">
+        <v>-17.30785389020097</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.1318433538228847</v>
+      </c>
+      <c r="D37" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>-6.426561576173299</v>
+      </c>
+      <c r="B38" t="n">
+        <v>-18.14236874156882</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-1.628389693210748</v>
+      </c>
+      <c r="D38" t="n">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>-7.253838026279618</v>
+      </c>
+      <c r="B39" t="n">
+        <v>-18.97688359293666</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-3.486622740244381</v>
+      </c>
+      <c r="D39" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>-8.081114476385936</v>
+      </c>
+      <c r="B40" t="n">
+        <v>-19.8113984443045</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-5.442855787278013</v>
+      </c>
+      <c r="D40" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>-8.908390926492256</v>
+      </c>
+      <c r="B41" t="n">
+        <v>-20.64591329567234</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-7.497088834311645</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>